<commit_message>
Name, description column length increased
</commit_message>
<xml_diff>
--- a/Importer.xlsx
+++ b/Importer.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -94,13 +94,424 @@
   </si>
   <si>
     <t>Nokia Mobile 1100</t>
+  </si>
+  <si>
+    <t>Nokia Mobile 3300</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/31/Nokia_3310_blue.jpg/1200px-Nokia_3310_blue.jpg</t>
+  </si>
+  <si>
+    <t>Tata Salt, 1 KG</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61j0wPsKqoL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Tata Sampann Unpolished Toor Dal/Arhar Dal, 1kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61XxbJq2nJL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Oats</t>
+  </si>
+  <si>
+    <t>Quaker Oats - 1.5 kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/810k%2BHT6MZL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Saffola Masala Oats, Classic Masala, 500g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/71bei6HanZL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Disano Oats with High in Protein and Fibre Pouch, 2 kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/71bgDvJVZHL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Kellogg's Corn Flakes Original, 1.2 kg</t>
+  </si>
+  <si>
+    <t>Flakes</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71d6lFe2WML._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Bagrry's Corn Flakes, 800g (with Extra 80g)</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81mBSoS6ibL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Nestle Everyday Dairy Whitener, Milk Powder for Tea, 1Kg Pouch</t>
+  </si>
+  <si>
+    <t>Coffee, Tea &amp; Beverages</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/7181KOQX05L._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Brooke Bond, Taj Mahal Tea, 500g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/71eyIBjj5DL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Dabur Hommade Coconut Milk- Goodness of 2 Creamy Coconuts-200 ml</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/71e4WbH6nwL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Cadbury Hot Chocolate Drink Powder Mix, 200 gm Pack</t>
+  </si>
+  <si>
+    <t>Hot Chocolate &amp; Malted Drinks</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/614An6eEFrL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Soyvita Enriched Soy Beverage Powder (Sweetened Regular Malt, 500gm)</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61HCcuHTQRL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Ovaltine Malt Beverage Mix (400 g) and Silver Plated Coin Combo</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/41RZ1nEY6gL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Rice, Flour &amp; Pulses</t>
+  </si>
+  <si>
+    <t>Tata Sampann Green Moong, Whole, 500g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61%2BzV82hJpL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Kohinoor Super Silver Aged Basmati Rice,5kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61VGYi4fkzL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Daawat Rozana Super Basmati Rice, 5kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81eyJQw4VNL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Sri Sri Tatttva Red Rice -1 Kg</t>
+  </si>
+  <si>
+    <t>Red Rice</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/91ZrjzQ9L0L._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Original Indian Table Mapillai Samba Red Rice, 1.25Kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81mqFhWnxxL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Dark Fantasy Choco Fills, 300g</t>
+  </si>
+  <si>
+    <t>Biscuits &amp; Cookies</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/51qHxF-NgsL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Sunfeast Mom's Magic Cashew and Almond, 600g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/819bDz6Q9DL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Parle-g Original Glucose Biscuit, 800g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/91eC2O5IN5L._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Cadbury Original Oreo Chocolatey Sandwich Biscuit Family Pack, 300g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/719zds2RDVL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Parle Krackjack Biscuit, 200g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81kcTKHwmoL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Parle Rusk, Elachi, 273g</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/51HWzaGKvAL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Bingo Mad Angles Tomato Madness Namkeen, 36.5g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81CTITd4iNL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Pickles</t>
+  </si>
+  <si>
+    <t>Add Me Home Made Dry Mango Pickle Less Oil 500gm Aam ka Achar Glass jar</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/91zyVe7inbL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Pachranga’s Farm Fresh Mixed Pickle - 1 kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/61PzWykoV9L._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Sun Grow Organic Homemade Stuffed Banarasi Red Chilli Pickle Achaar ( Taste of Banaras )</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81OabtTm5RL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Dried Fruits, Nuts &amp; Seeds</t>
+  </si>
+  <si>
+    <t>Happilo 100% Natural Premium Californian Almonds, 200g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/81PcJl7XviL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Amazon Brand - Vedaka Popular Whole Almonds, 1kg</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/91WuE6fxVtL._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>Happilo Premium Seedless Green Raisins, 250g</t>
+  </si>
+  <si>
+    <t>https://images-eu.ssl-images-amazon.com/images/I/91OIuJLCq8L._AC_UL200_SR200,200_.jpg</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>Cauliflower</t>
+  </si>
+  <si>
+    <t>Capsicum</t>
+  </si>
+  <si>
+    <t>https://www.naturefresh.ca/wp-content/uploads/NFF-health-benefits-of-Tomatoes.jpg</t>
+  </si>
+  <si>
+    <t>https://www.sentinelassam.com/wp-content/uploads/2018/08/Cabbage.png</t>
+  </si>
+  <si>
+    <t>https://cdn.theatlantic.com/thumbor/TxEw_yjPER1uluJjP8qc0nNRHpw=/0x72:1000x635/720x405/media/img/mt/2015/05/shutterstock_247399801/original.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn-b.medlife.com/2019/04/cucumber-health-benefits.png</t>
+  </si>
+  <si>
+    <t>https://www.tasteofhome.com/wp-content/uploads/2019/01/carrots-shutterstock_789443206.jpg</t>
+  </si>
+  <si>
+    <t>https://bakingmischief.com/wp-content/uploads/2018/06/how-to-steam-green-beans-in-the-microwave-image-square-500x375.jpg</t>
+  </si>
+  <si>
+    <t>https://snaped.fns.usda.gov/sites/default/files/styles/crop_ratio_7_5/public/seasonal-produce/2018-05/pumpkin.jpg?itok=IXGgRg1X</t>
+  </si>
+  <si>
+    <t>https://cms.splendidtable.org/sites/default/files/styles/w2000/public/sugarsnappeas.jpg?itok=sMoAZWdi</t>
+  </si>
+  <si>
+    <t>https://thumbor.forbes.com/thumbor/960x0/https%3A%2F%2Fspecials-images.forbesimg.com%2Fdam%2Fimageserve%2F1136653496%2F960x0.jpg%3Ffit%3Dscale</t>
+  </si>
+  <si>
+    <t>https://www.acouplecooks.com/wp-content/uploads/2019/10/Beet-Salad-001.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/41F62-VbHSL._SX425_.jpg</t>
+  </si>
+  <si>
+    <t>https://pcdn.columbian.com/wp-content/uploads/2019/07/0726_WKD_market-fresh-Cauliflower-1226x0-c-default.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/31RHnbD8xlL._SX466_.jpg</t>
+  </si>
+  <si>
+    <t>https://img.manoramaonline.com/content/dam/mm/en/lifestyle/health/images/2019/2/22/garlic-c.jpg</t>
+  </si>
+  <si>
+    <t>https://i.ytimg.com/vi/47uyWsTcOa8/maxresdefault.jpg</t>
+  </si>
+  <si>
+    <t>https://imgk.timesnownews.com/story/ginger-benefits.gif?tr=w-1200,h-900</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71ptno4aB1L._SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>Lemon 250gm</t>
+  </si>
+  <si>
+    <t>Potato 1KG</t>
+  </si>
+  <si>
+    <t>Carrot 500gm</t>
+  </si>
+  <si>
+    <t>Beetroot 500gm</t>
+  </si>
+  <si>
+    <t>Green Beans 500gm</t>
+  </si>
+  <si>
+    <t>Ginger 250gm</t>
+  </si>
+  <si>
+    <t>Onion 1KG</t>
+  </si>
+  <si>
+    <t>Pumpkin 500gm</t>
+  </si>
+  <si>
+    <t>Cucumber 500gm</t>
+  </si>
+  <si>
+    <t>Tomato 1KG</t>
+  </si>
+  <si>
+    <t>Corn 200gm</t>
+  </si>
+  <si>
+    <t>Garlic 250gm</t>
+  </si>
+  <si>
+    <t>Peas 500gm</t>
+  </si>
+  <si>
+    <t>Mushroom 250gm</t>
+  </si>
+  <si>
+    <t>Yam Elephant 500gm</t>
+  </si>
+  <si>
+    <t>Ash Gourd 500gm</t>
+  </si>
+  <si>
+    <t>Green Plantain 500gm</t>
+  </si>
+  <si>
+    <t>Drumstick 500gm</t>
+  </si>
+  <si>
+    <t>Ladies Finger 250gm</t>
+  </si>
+  <si>
+    <t>Brinjal 500gm</t>
+  </si>
+  <si>
+    <t>Coconut</t>
+  </si>
+  <si>
+    <t>Green Chillies 150gm</t>
+  </si>
+  <si>
+    <t>Coriender Leaves 100gm</t>
+  </si>
+  <si>
+    <t>Mint Leaves 100gm</t>
+  </si>
+  <si>
+    <t>Curry Leaves</t>
+  </si>
+  <si>
+    <t>Bitter Gourd 250gm</t>
+  </si>
+  <si>
+    <t>Radish White 250gm</t>
+  </si>
+  <si>
+    <t>Green Palak 1 Pack</t>
+  </si>
+  <si>
+    <t>https://5.imimg.com/data5/OK/IT/GLADMIN-30212742/fresh-elephant-foot-yam-500x500.png</t>
+  </si>
+  <si>
+    <t>https://equiposwalker.com/wp-content/uploads/2017/08/815-800x379.png?9d7bd4&amp;9d7bd4</t>
+  </si>
+  <si>
+    <t>https://www.netmeds.com/images/cms/wysiwyg/blog/2020/03/1584520187_AshGourd_big_3.jpg</t>
+  </si>
+  <si>
+    <t>https://sc01.alicdn.com/kf/UTB84zhjMVfFXKJk43Otq6xIPFXat/949253968/UTB84zhjMVfFXKJk43Otq6xIPFXat.jpg</t>
+  </si>
+  <si>
+    <t>https://anandhagrocery.com/wp-content/uploads/2019/02/lady-fingers-vendakkai.jpg</t>
+  </si>
+  <si>
+    <t>https://image.shutterstock.com/image-photo/egg-plant-isolated-on-white-260nw-280847201.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/grohealth/image/upload/f_auto,fl_lossy,q_auto/v1581688797/DCUK/Content/Coconut-Cooking-Oil-Food-And-Drink-Coco-Close-up_Medium.jpg</t>
+  </si>
+  <si>
+    <t>https://paramanfoodworks.com/store/91-large_default/coriander-leaves-powder-100-gms.jpg</t>
+  </si>
+  <si>
+    <t>https://5.imimg.com/data5/QH/BV/GLADMIN-36212634/mint-leaves-powder-500x500.png</t>
+  </si>
+  <si>
+    <t>https://vaya.in/news/wp-content/uploads/2019/03/curry-leaves-1280x720.jpg</t>
+  </si>
+  <si>
+    <t>https://www.deccanherald.com/sites/dh/files/styles/article_detail/public/article_images/2019/05/28/file70ypwbq2rvmddu4ke62-1558985401.jpg?itok=vvQ41pUz</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/originals/60/a6/eb/60a6eb7e61e996d1907e139b74649f06.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/51HTxtejpDL._SX466_.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +549,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,41 +584,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -322,6 +726,28 @@
         <outline val="0"/>
         <shadow val="0"/>
         <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
         <sz val="9"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -341,27 +767,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Items" displayName="Items" ref="A1:F5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="7">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Items" displayName="Items" ref="A1:F70" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:F70"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Category Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Price" dataDxfId="9"/>
-    <tableColumn id="4" name="Selling" dataDxfId="8"/>
-    <tableColumn id="5" name="Stock" dataDxfId="1"/>
-    <tableColumn id="6" name="Image Link" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name" dataDxfId="10"/>
+    <tableColumn id="2" name="Category Name" dataDxfId="9"/>
+    <tableColumn id="3" name="Price" dataDxfId="8"/>
+    <tableColumn id="4" name="Selling" dataDxfId="7"/>
+    <tableColumn id="5" name="Stock" dataDxfId="6"/>
+    <tableColumn id="6" name="Image Link" dataDxfId="5" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Categories" displayName="Categories" ref="A1:C5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Categories" displayName="Categories" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name " dataDxfId="5"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Image" dataDxfId="2"/>
+    <tableColumn id="1" name="Name " dataDxfId="2"/>
+    <tableColumn id="2" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" name="Image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,20 +1056,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -742,6 +1168,1285 @@
         <v>7</v>
       </c>
       <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3200</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2">
+        <v>125</v>
+      </c>
+      <c r="D9" s="2">
+        <v>125</v>
+      </c>
+      <c r="E9" s="2">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2">
+        <v>249</v>
+      </c>
+      <c r="D10" s="2">
+        <v>249</v>
+      </c>
+      <c r="E10" s="2">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2">
+        <v>180</v>
+      </c>
+      <c r="D11" s="2">
+        <v>180</v>
+      </c>
+      <c r="E11" s="2">
+        <v>40</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2">
+        <v>289</v>
+      </c>
+      <c r="D12" s="2">
+        <v>289</v>
+      </c>
+      <c r="E12" s="2">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2">
+        <v>379</v>
+      </c>
+      <c r="D13" s="2">
+        <v>379</v>
+      </c>
+      <c r="E13" s="2">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>330</v>
+      </c>
+      <c r="D14" s="2">
+        <v>330</v>
+      </c>
+      <c r="E14" s="2">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2">
+        <v>487</v>
+      </c>
+      <c r="D15" s="2">
+        <v>487</v>
+      </c>
+      <c r="E15" s="2">
+        <v>40</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2">
+        <v>305</v>
+      </c>
+      <c r="D16" s="2">
+        <v>305</v>
+      </c>
+      <c r="E16" s="2">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2">
+        <v>71</v>
+      </c>
+      <c r="D17" s="2">
+        <v>71</v>
+      </c>
+      <c r="E17" s="2">
+        <v>40</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2">
+        <v>210</v>
+      </c>
+      <c r="D18" s="2">
+        <v>210</v>
+      </c>
+      <c r="E18" s="2">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2">
+        <v>390</v>
+      </c>
+      <c r="D19" s="2">
+        <v>390</v>
+      </c>
+      <c r="E19" s="2">
+        <v>40</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2">
+        <v>440</v>
+      </c>
+      <c r="D20" s="2">
+        <v>440</v>
+      </c>
+      <c r="E20" s="2">
+        <v>40</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2">
+        <v>76</v>
+      </c>
+      <c r="E21" s="2">
+        <v>40</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2">
+        <v>519</v>
+      </c>
+      <c r="D22" s="2">
+        <v>519</v>
+      </c>
+      <c r="E22" s="2">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2">
+        <v>329</v>
+      </c>
+      <c r="D23" s="2">
+        <v>329</v>
+      </c>
+      <c r="E23" s="2">
+        <v>40</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2">
+        <v>130</v>
+      </c>
+      <c r="D24" s="2">
+        <v>130</v>
+      </c>
+      <c r="E24" s="2">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2">
+        <v>260</v>
+      </c>
+      <c r="D25" s="2">
+        <v>260</v>
+      </c>
+      <c r="E25" s="2">
+        <v>40</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="2">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2">
+        <v>96</v>
+      </c>
+      <c r="E26" s="2">
+        <v>40</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="2">
+        <v>94.5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>94.5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>40</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2">
+        <v>69</v>
+      </c>
+      <c r="E28" s="2">
+        <v>40</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="2">
+        <v>75</v>
+      </c>
+      <c r="D29" s="2">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2">
+        <v>40</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2">
+        <v>30</v>
+      </c>
+      <c r="E30" s="2">
+        <v>40</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="2">
+        <v>35</v>
+      </c>
+      <c r="D31" s="2">
+        <v>35</v>
+      </c>
+      <c r="E31" s="2">
+        <v>40</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2">
+        <v>25</v>
+      </c>
+      <c r="E32" s="2">
+        <v>40</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="2">
+        <v>320</v>
+      </c>
+      <c r="D33" s="2">
+        <v>320</v>
+      </c>
+      <c r="E33" s="2">
+        <v>40</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="2">
+        <v>140</v>
+      </c>
+      <c r="D34" s="2">
+        <v>140</v>
+      </c>
+      <c r="E34" s="2">
+        <v>40</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="2">
+        <v>380</v>
+      </c>
+      <c r="D35" s="2">
+        <v>380</v>
+      </c>
+      <c r="E35" s="2">
+        <v>40</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="2">
+        <v>220</v>
+      </c>
+      <c r="D36" s="2">
+        <v>220</v>
+      </c>
+      <c r="E36" s="2">
+        <v>40</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2">
+        <v>949</v>
+      </c>
+      <c r="D37" s="2">
+        <v>949</v>
+      </c>
+      <c r="E37" s="2">
+        <v>40</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="2">
+        <v>156</v>
+      </c>
+      <c r="D38" s="2">
+        <v>156</v>
+      </c>
+      <c r="E38" s="2">
+        <v>40</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="6">
+        <v>25</v>
+      </c>
+      <c r="D40" s="6">
+        <v>25</v>
+      </c>
+      <c r="E40" s="6">
+        <v>40</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="6">
+        <v>45</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45</v>
+      </c>
+      <c r="E41" s="6">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="6">
+        <v>30</v>
+      </c>
+      <c r="D42" s="6">
+        <v>30</v>
+      </c>
+      <c r="E42" s="6">
+        <v>40</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="6">
+        <v>65</v>
+      </c>
+      <c r="D43" s="6">
+        <v>65</v>
+      </c>
+      <c r="E43" s="6">
+        <v>40</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="D44" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="E44" s="6">
+        <v>40</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="6">
+        <v>32.5</v>
+      </c>
+      <c r="D45" s="6">
+        <v>32.5</v>
+      </c>
+      <c r="E45" s="6">
+        <v>40</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="6">
+        <v>125</v>
+      </c>
+      <c r="D46" s="6">
+        <v>125</v>
+      </c>
+      <c r="E46" s="6">
+        <v>40</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="D47" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="E47" s="6">
+        <v>40</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="D48" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="E48" s="6">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="6">
+        <v>60</v>
+      </c>
+      <c r="D49" s="6">
+        <v>60</v>
+      </c>
+      <c r="E49" s="6">
+        <v>40</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="6">
+        <v>30</v>
+      </c>
+      <c r="D50" s="6">
+        <v>30</v>
+      </c>
+      <c r="E50" s="6">
+        <v>40</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="6">
+        <v>55</v>
+      </c>
+      <c r="D51" s="6">
+        <v>55</v>
+      </c>
+      <c r="E51" s="6">
+        <v>40</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="6">
+        <v>35</v>
+      </c>
+      <c r="D52" s="6">
+        <v>35</v>
+      </c>
+      <c r="E52" s="6">
+        <v>40</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="D53" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="E53" s="6">
+        <v>40</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="6">
+        <v>60</v>
+      </c>
+      <c r="D54" s="6">
+        <v>60</v>
+      </c>
+      <c r="E54" s="6">
+        <v>40</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="6">
+        <v>10</v>
+      </c>
+      <c r="D55" s="6">
+        <v>10</v>
+      </c>
+      <c r="E55" s="6">
+        <v>40</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="6">
+        <v>30</v>
+      </c>
+      <c r="D56" s="6">
+        <v>30</v>
+      </c>
+      <c r="E56" s="6">
+        <v>40</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="D57" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="E57" s="6">
+        <v>40</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="6">
+        <v>25</v>
+      </c>
+      <c r="D58" s="6">
+        <v>25</v>
+      </c>
+      <c r="E58" s="6">
+        <v>40</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="D59" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="E59" s="6">
+        <v>40</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="6">
+        <v>23</v>
+      </c>
+      <c r="D60" s="6">
+        <v>23</v>
+      </c>
+      <c r="E60" s="6">
+        <v>40</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="6">
+        <v>38</v>
+      </c>
+      <c r="D61" s="6">
+        <v>38</v>
+      </c>
+      <c r="E61" s="6">
+        <v>40</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="6">
+        <v>15</v>
+      </c>
+      <c r="D62" s="6">
+        <v>15</v>
+      </c>
+      <c r="E62" s="6">
+        <v>40</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" s="6">
+        <v>25</v>
+      </c>
+      <c r="D63" s="6">
+        <v>25</v>
+      </c>
+      <c r="E63" s="6">
+        <v>40</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="6">
+        <v>30</v>
+      </c>
+      <c r="D64" s="6">
+        <v>30</v>
+      </c>
+      <c r="E64" s="6">
+        <v>40</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="6">
+        <v>25</v>
+      </c>
+      <c r="D65" s="6">
+        <v>25</v>
+      </c>
+      <c r="E65" s="6">
+        <v>40</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="6">
+        <v>8</v>
+      </c>
+      <c r="D66" s="6">
+        <v>8</v>
+      </c>
+      <c r="E66" s="6">
+        <v>40</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1</v>
+      </c>
+      <c r="D67" s="6">
+        <v>1</v>
+      </c>
+      <c r="E67" s="6">
+        <v>40</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C68" s="6">
+        <v>15</v>
+      </c>
+      <c r="D68" s="6">
+        <v>15</v>
+      </c>
+      <c r="E68" s="6">
+        <v>40</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="D69" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="E69" s="6">
+        <v>40</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" s="6">
+        <v>15</v>
+      </c>
+      <c r="D70" s="6">
+        <v>15</v>
+      </c>
+      <c r="E70" s="6">
+        <v>40</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>